<commit_message>
Minor changes on Ctrl class & UML
</commit_message>
<xml_diff>
--- a/Evaluation Grid.xlsx
+++ b/Evaluation Grid.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Desktop\PROJET JAVA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Documents\GitHub\BoulderDashProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -385,7 +385,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +398,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -787,20 +799,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -892,6 +892,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -919,11 +937,21 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1212,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:S4"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,1033 +1254,1033 @@
   <sheetData>
     <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:23" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="3" t="str">
+      <c r="A4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="34" t="str">
         <f>IF(X4&gt;=(C6*I6*O6*U6)*0.7,"A",IF(AD4&gt;=(C6*I6*O6*U6)*0.5,"B",IF(AD4&gt;=(C6*I6*O6*U6)*0.3,"C","D")))</f>
         <v>D</v>
       </c>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="4"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="35"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="7"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="3"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="3"/>
     </row>
     <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2">
         <f>IF(B7="A",4,IF(B7="B",3,IF(B7="C",1,0)))</f>
         <v>0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="H6" s="6">
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="H6" s="2">
         <f>IF(H7="A",4,IF(H7="B",3,IF(H7="C",1,0)))</f>
         <v>0</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="3">
         <v>4</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-      <c r="N6" s="6">
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="N6" s="2">
         <f>IF(N7="A",4,IF(N7="B",3,IF(N7="C",1,0)))</f>
         <v>0</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="2">
         <v>4</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="7"/>
-      <c r="T6" s="6">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="3"/>
+      <c r="T6" s="2">
         <f>IF(T7="A",4,IF(T7="B",3,IF(T7="C",1,0)))</f>
         <v>0</v>
       </c>
-      <c r="U6" s="6">
-        <v>1</v>
-      </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="7"/>
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9" t="str">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="str">
         <f>IF(D7&gt;SUM(C8:C22)*0.7,"A",IF(D7&gt;=SUM(C8:C22)*0.5,"B",IF(D7&gt;=SUM(C8:C22)*0.3,"C","D")))</f>
         <v>D</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="C7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5">
         <f>SUM(D8:D24)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="12" t="str">
+      <c r="H7" s="8" t="str">
         <f>IF(J7&gt;SUM(I8:I24)*0.7,"A",IF(J7&gt;=SUM(I8:I24)*0.5,"B",IF(J7&gt;=SUM(I8:I24)*0.3,"C","D")))</f>
         <v>D</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="I7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="9">
         <f>SUM(J8:J24)</f>
         <v>0</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11" t="s">
+      <c r="L7" s="6"/>
+      <c r="M7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="12" t="str">
+      <c r="N7" s="8" t="str">
         <f>IF(P7&gt;SUM(O8:O16)*0.7,"A",IF(P7&gt;=SUM(O8:O16)*0.5,"B",IF(P7&gt;=SUM(O8:O16)*0.3,"C","D")))</f>
         <v>D</v>
       </c>
-      <c r="O7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="12">
+      <c r="O7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="8">
         <f>SUM(P8:P17)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="13" t="s">
+      <c r="Q7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="11" t="s">
+      <c r="R7" s="6"/>
+      <c r="S7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="T7" s="12" t="str">
+      <c r="T7" s="8" t="str">
         <f>IF(PRODUCT(V8:V17),"A","D")</f>
         <v>D</v>
       </c>
-      <c r="U7" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="12">
+      <c r="U7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="8">
         <f>PRODUCT(V8:V17)</f>
         <v>0</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16">
-        <v>2</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12">
         <f>(B8/E8)*C8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="12">
         <v>5</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="20">
+      <c r="H8" s="15"/>
+      <c r="I8" s="16">
         <v>3</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="17">
         <f>(H8/K8)*I8</f>
         <v>0</v>
       </c>
-      <c r="K8" s="22">
-        <v>2</v>
-      </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="18" t="s">
+      <c r="K8" s="18">
+        <v>2</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="19"/>
-      <c r="O8" s="20">
+      <c r="N8" s="15"/>
+      <c r="O8" s="16">
         <v>3</v>
       </c>
-      <c r="P8" s="20">
+      <c r="P8" s="16">
         <f>(N8/Q8)*O8</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="23">
-        <v>2</v>
-      </c>
-      <c r="R8" s="17"/>
-      <c r="S8" s="18" t="s">
+      <c r="Q8" s="19">
+        <v>2</v>
+      </c>
+      <c r="R8" s="13"/>
+      <c r="S8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="T8" s="19"/>
-      <c r="U8" s="20">
-        <v>1</v>
-      </c>
-      <c r="V8" s="20">
+      <c r="T8" s="45"/>
+      <c r="U8" s="16">
+        <v>1</v>
+      </c>
+      <c r="V8" s="16">
         <f>(T8/W8)*U8</f>
         <v>0</v>
       </c>
-      <c r="W8" s="23">
+      <c r="W8" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26">
-        <v>2</v>
-      </c>
-      <c r="D9" s="26">
+      <c r="B9" s="21"/>
+      <c r="C9" s="22">
+        <v>2</v>
+      </c>
+      <c r="D9" s="22">
         <f t="shared" ref="D9:D22" si="0">(B9/E9)*C9</f>
         <v>0</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="22">
         <v>4</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="24" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26">
+      <c r="H9" s="21"/>
+      <c r="I9" s="22">
         <v>3</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="23">
         <f t="shared" ref="J9:J24" si="1">(H9/K9)*I9</f>
         <v>0</v>
       </c>
-      <c r="K9" s="28">
-        <v>1</v>
-      </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="24" t="s">
+      <c r="K9" s="24">
+        <v>1</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="26">
+      <c r="N9" s="21"/>
+      <c r="O9" s="22">
         <v>3</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="22">
         <f t="shared" ref="P9:P17" si="2">(N9/Q9)*O9</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="29">
-        <v>1</v>
-      </c>
-      <c r="R9" s="17"/>
-      <c r="S9" s="24" t="s">
+      <c r="Q9" s="25">
+        <v>1</v>
+      </c>
+      <c r="R9" s="13"/>
+      <c r="S9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="25"/>
-      <c r="U9" s="26">
-        <v>1</v>
-      </c>
-      <c r="V9" s="26">
+      <c r="T9" s="47"/>
+      <c r="U9" s="22">
+        <v>1</v>
+      </c>
+      <c r="V9" s="22">
         <f t="shared" ref="V9:V17" si="3">(T9/W9)*U9</f>
         <v>0</v>
       </c>
-      <c r="W9" s="29">
+      <c r="W9" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22">
         <v>3</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E10" s="26">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="24" t="s">
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26">
-        <v>2</v>
-      </c>
-      <c r="J10" s="27">
+      <c r="H10" s="21"/>
+      <c r="I10" s="22">
+        <v>2</v>
+      </c>
+      <c r="J10" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="28">
-        <v>2</v>
-      </c>
-      <c r="L10" s="17"/>
-      <c r="M10" s="24" t="s">
+      <c r="K10" s="24">
+        <v>2</v>
+      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="25"/>
-      <c r="O10" s="26">
-        <v>2</v>
-      </c>
-      <c r="P10" s="26">
+      <c r="N10" s="21"/>
+      <c r="O10" s="22">
+        <v>2</v>
+      </c>
+      <c r="P10" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="29">
-        <v>1</v>
-      </c>
-      <c r="R10" s="17"/>
-      <c r="S10" s="24" t="s">
+      <c r="Q10" s="25">
+        <v>1</v>
+      </c>
+      <c r="R10" s="13"/>
+      <c r="S10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="T10" s="25"/>
-      <c r="U10" s="26">
-        <v>1</v>
-      </c>
-      <c r="V10" s="26">
+      <c r="T10" s="47"/>
+      <c r="U10" s="22">
+        <v>1</v>
+      </c>
+      <c r="V10" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W10" s="29">
+      <c r="W10" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22">
         <v>3</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="26">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="24" t="s">
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26">
+      <c r="H11" s="21"/>
+      <c r="I11" s="22">
         <v>3</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K11" s="28">
-        <v>2</v>
-      </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="24" t="s">
+      <c r="K11" s="24">
+        <v>2</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="26">
-        <v>2</v>
-      </c>
-      <c r="P11" s="26">
+      <c r="N11" s="21"/>
+      <c r="O11" s="22">
+        <v>2</v>
+      </c>
+      <c r="P11" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="29">
-        <v>1</v>
-      </c>
-      <c r="R11" s="17"/>
-      <c r="S11" s="24" t="s">
+      <c r="Q11" s="25">
+        <v>1</v>
+      </c>
+      <c r="R11" s="13"/>
+      <c r="S11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="25"/>
-      <c r="U11" s="26">
-        <v>1</v>
-      </c>
-      <c r="V11" s="26">
+      <c r="T11" s="47"/>
+      <c r="U11" s="22">
+        <v>1</v>
+      </c>
+      <c r="V11" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W11" s="29">
+      <c r="W11" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26">
-        <v>2</v>
-      </c>
-      <c r="D12" s="26">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22">
+        <v>2</v>
+      </c>
+      <c r="D12" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E12" s="26">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="24" t="s">
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="26">
-        <v>2</v>
-      </c>
-      <c r="J12" s="27">
+      <c r="H12" s="21"/>
+      <c r="I12" s="22">
+        <v>2</v>
+      </c>
+      <c r="J12" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K12" s="28">
-        <v>2</v>
-      </c>
-      <c r="L12" s="17"/>
-      <c r="M12" s="24" t="s">
+      <c r="K12" s="24">
+        <v>2</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="26">
-        <v>2</v>
-      </c>
-      <c r="P12" s="26">
+      <c r="N12" s="21"/>
+      <c r="O12" s="22">
+        <v>2</v>
+      </c>
+      <c r="P12" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="29">
-        <v>2</v>
-      </c>
-      <c r="R12" s="17"/>
-      <c r="S12" s="24" t="s">
+      <c r="Q12" s="25">
+        <v>2</v>
+      </c>
+      <c r="R12" s="13"/>
+      <c r="S12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="25"/>
-      <c r="U12" s="26">
-        <v>1</v>
-      </c>
-      <c r="V12" s="26">
+      <c r="T12" s="47"/>
+      <c r="U12" s="22">
+        <v>1</v>
+      </c>
+      <c r="V12" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W12" s="29">
+      <c r="W12" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22">
         <v>3</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E13" s="26">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="24" t="s">
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26">
+      <c r="H13" s="21"/>
+      <c r="I13" s="22">
         <v>3</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K13" s="28">
-        <v>1</v>
-      </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="24" t="s">
+      <c r="K13" s="24">
+        <v>1</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="26">
-        <v>2</v>
-      </c>
-      <c r="P13" s="26">
+      <c r="N13" s="21"/>
+      <c r="O13" s="22">
+        <v>2</v>
+      </c>
+      <c r="P13" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="29">
-        <v>2</v>
-      </c>
-      <c r="R13" s="17"/>
-      <c r="S13" s="24" t="s">
+      <c r="Q13" s="25">
+        <v>2</v>
+      </c>
+      <c r="R13" s="13"/>
+      <c r="S13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="T13" s="25"/>
-      <c r="U13" s="26">
-        <v>1</v>
-      </c>
-      <c r="V13" s="26">
+      <c r="T13" s="47"/>
+      <c r="U13" s="22">
+        <v>1</v>
+      </c>
+      <c r="V13" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W13" s="29">
+      <c r="W13" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22">
         <v>3</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" s="26">
-        <v>1</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="24" t="s">
+      <c r="E14" s="22">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26">
+      <c r="H14" s="21"/>
+      <c r="I14" s="22">
         <v>3</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K14" s="28">
-        <v>1</v>
-      </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="24" t="s">
+      <c r="K14" s="24">
+        <v>1</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="25"/>
-      <c r="O14" s="26">
-        <v>2</v>
-      </c>
-      <c r="P14" s="26">
+      <c r="N14" s="21"/>
+      <c r="O14" s="22">
+        <v>2</v>
+      </c>
+      <c r="P14" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="29">
-        <v>2</v>
-      </c>
-      <c r="R14" s="17"/>
-      <c r="S14" s="24" t="s">
+      <c r="Q14" s="25">
+        <v>2</v>
+      </c>
+      <c r="R14" s="13"/>
+      <c r="S14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="T14" s="25"/>
-      <c r="U14" s="26">
-        <v>1</v>
-      </c>
-      <c r="V14" s="26">
+      <c r="T14" s="46"/>
+      <c r="U14" s="22">
+        <v>1</v>
+      </c>
+      <c r="V14" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W14" s="29">
+      <c r="W14" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="26">
-        <v>2</v>
-      </c>
-      <c r="D15" s="26">
+      <c r="B15" s="21"/>
+      <c r="C15" s="22">
+        <v>2</v>
+      </c>
+      <c r="D15" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15" s="26">
-        <v>1</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="24" t="s">
+      <c r="E15" s="22">
+        <v>1</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="26">
+      <c r="H15" s="21"/>
+      <c r="I15" s="22">
         <v>3</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K15" s="28">
-        <v>1</v>
-      </c>
-      <c r="L15" s="17"/>
-      <c r="M15" s="24" t="s">
+      <c r="K15" s="24">
+        <v>1</v>
+      </c>
+      <c r="L15" s="13"/>
+      <c r="M15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="N15" s="25"/>
-      <c r="O15" s="26">
-        <v>2</v>
-      </c>
-      <c r="P15" s="26">
+      <c r="N15" s="21"/>
+      <c r="O15" s="22">
+        <v>2</v>
+      </c>
+      <c r="P15" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="29">
-        <v>1</v>
-      </c>
-      <c r="R15" s="17"/>
-      <c r="S15" s="24" t="s">
+      <c r="Q15" s="25">
+        <v>1</v>
+      </c>
+      <c r="R15" s="13"/>
+      <c r="S15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="T15" s="25"/>
-      <c r="U15" s="26">
-        <v>1</v>
-      </c>
-      <c r="V15" s="26">
+      <c r="T15" s="46"/>
+      <c r="U15" s="22">
+        <v>1</v>
+      </c>
+      <c r="V15" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W15" s="29">
+      <c r="W15" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="99" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26">
-        <v>1</v>
-      </c>
-      <c r="D16" s="26">
+      <c r="B16" s="21"/>
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+      <c r="D16" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E16" s="26">
-        <v>1</v>
-      </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="24" t="s">
+      <c r="E16" s="22">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22">
         <v>3</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K16" s="28">
-        <v>1</v>
-      </c>
-      <c r="L16" s="17"/>
-      <c r="M16" s="24" t="s">
+      <c r="K16" s="24">
+        <v>1</v>
+      </c>
+      <c r="L16" s="13"/>
+      <c r="M16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="N16" s="25"/>
-      <c r="O16" s="26">
-        <v>2</v>
-      </c>
-      <c r="P16" s="26">
+      <c r="N16" s="21"/>
+      <c r="O16" s="22">
+        <v>2</v>
+      </c>
+      <c r="P16" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="29">
-        <v>2</v>
-      </c>
-      <c r="R16" s="17"/>
-      <c r="S16" s="24" t="s">
+      <c r="Q16" s="25">
+        <v>2</v>
+      </c>
+      <c r="R16" s="13"/>
+      <c r="S16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="T16" s="25"/>
-      <c r="U16" s="26">
-        <v>1</v>
-      </c>
-      <c r="V16" s="26">
+      <c r="T16" s="46"/>
+      <c r="U16" s="22">
+        <v>1</v>
+      </c>
+      <c r="V16" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W16" s="29">
+      <c r="W16" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26">
+      <c r="B17" s="21"/>
+      <c r="C17" s="22">
         <v>3</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E17" s="26">
-        <v>1</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="24" t="s">
+      <c r="E17" s="22">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26">
-        <v>2</v>
-      </c>
-      <c r="J17" s="27">
+      <c r="H17" s="21"/>
+      <c r="I17" s="22">
+        <v>2</v>
+      </c>
+      <c r="J17" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K17" s="28">
-        <v>2</v>
-      </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="30" t="s">
+      <c r="K17" s="24">
+        <v>2</v>
+      </c>
+      <c r="L17" s="13"/>
+      <c r="M17" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="31"/>
-      <c r="O17" s="32">
+      <c r="N17" s="27"/>
+      <c r="O17" s="28">
         <v>3</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="33">
+      <c r="Q17" s="29">
         <v>3</v>
       </c>
-      <c r="R17" s="17"/>
-      <c r="S17" s="30" t="s">
+      <c r="R17" s="13"/>
+      <c r="S17" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="T17" s="31"/>
-      <c r="U17" s="32">
-        <v>1</v>
-      </c>
-      <c r="V17" s="32">
+      <c r="T17" s="48"/>
+      <c r="U17" s="28">
+        <v>1</v>
+      </c>
+      <c r="V17" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W17" s="33">
+      <c r="W17" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26">
-        <v>2</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="B18" s="21"/>
+      <c r="C18" s="22">
+        <v>2</v>
+      </c>
+      <c r="D18" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="26">
-        <v>1</v>
-      </c>
-      <c r="G18" s="24" t="s">
+      <c r="E18" s="22">
+        <v>1</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="26">
-        <v>2</v>
-      </c>
-      <c r="J18" s="27">
+      <c r="H18" s="21"/>
+      <c r="I18" s="22">
+        <v>2</v>
+      </c>
+      <c r="J18" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K18" s="28">
-        <v>2</v>
-      </c>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="7"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="7"/>
+      <c r="K18" s="24">
+        <v>2</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="3"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="3"/>
     </row>
     <row r="19" spans="1:23" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26">
-        <v>2</v>
-      </c>
-      <c r="D19" s="26">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22">
+        <v>2</v>
+      </c>
+      <c r="D19" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="26">
-        <v>1</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="E19" s="22">
+        <v>1</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26">
-        <v>2</v>
-      </c>
-      <c r="J19" s="27">
+      <c r="H19" s="21"/>
+      <c r="I19" s="22">
+        <v>2</v>
+      </c>
+      <c r="J19" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="28">
-        <v>2</v>
-      </c>
-      <c r="M19" s="34" t="s">
+      <c r="K19" s="24">
+        <v>2</v>
+      </c>
+      <c r="M19" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="36"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="38"/>
     </row>
     <row r="20" spans="1:23" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26">
-        <v>2</v>
-      </c>
-      <c r="D20" s="26">
+      <c r="B20" s="21"/>
+      <c r="C20" s="22">
+        <v>2</v>
+      </c>
+      <c r="D20" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="26">
-        <v>1</v>
-      </c>
-      <c r="G20" s="24" t="s">
+      <c r="E20" s="22">
+        <v>1</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26">
+      <c r="H20" s="21"/>
+      <c r="I20" s="22">
         <v>3</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K20" s="28">
-        <v>1</v>
-      </c>
-      <c r="M20" s="37"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="39"/>
+      <c r="K20" s="24">
+        <v>1</v>
+      </c>
+      <c r="M20" s="39"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="41"/>
     </row>
     <row r="21" spans="1:23" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26">
+      <c r="B21" s="21"/>
+      <c r="C21" s="22">
         <v>3</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="26">
-        <v>1</v>
-      </c>
-      <c r="G21" s="24" t="s">
+      <c r="E21" s="22">
+        <v>1</v>
+      </c>
+      <c r="G21" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26">
-        <v>1</v>
-      </c>
-      <c r="J21" s="27">
+      <c r="H21" s="21"/>
+      <c r="I21" s="22">
+        <v>1</v>
+      </c>
+      <c r="J21" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K21" s="28">
-        <v>2</v>
-      </c>
-      <c r="M21" s="37"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38"/>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="39"/>
+      <c r="K21" s="24">
+        <v>2</v>
+      </c>
+      <c r="M21" s="39"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="41"/>
     </row>
     <row r="22" spans="1:23" ht="46.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32">
-        <v>2</v>
-      </c>
-      <c r="D22" s="32">
+      <c r="B22" s="27"/>
+      <c r="C22" s="28">
+        <v>2</v>
+      </c>
+      <c r="D22" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="32">
-        <v>1</v>
-      </c>
-      <c r="G22" s="24" t="s">
+      <c r="E22" s="28">
+        <v>1</v>
+      </c>
+      <c r="G22" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="26">
+      <c r="H22" s="21"/>
+      <c r="I22" s="22">
         <v>3</v>
       </c>
-      <c r="J22" s="27">
+      <c r="J22" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K22" s="28">
-        <v>2</v>
-      </c>
-      <c r="M22" s="37"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="38"/>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="38"/>
-      <c r="U22" s="38"/>
-      <c r="V22" s="38"/>
-      <c r="W22" s="39"/>
+      <c r="K22" s="24">
+        <v>2</v>
+      </c>
+      <c r="M22" s="39"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
+      <c r="W22" s="41"/>
     </row>
     <row r="23" spans="1:23" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="G23" s="24" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="G23" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="26">
-        <v>1</v>
-      </c>
-      <c r="J23" s="27">
+      <c r="H23" s="21"/>
+      <c r="I23" s="22">
+        <v>1</v>
+      </c>
+      <c r="J23" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K23" s="28">
-        <v>2</v>
-      </c>
-      <c r="M23" s="40"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="41"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="42"/>
+      <c r="K23" s="24">
+        <v>2</v>
+      </c>
+      <c r="M23" s="42"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+      <c r="S23" s="43"/>
+      <c r="T23" s="43"/>
+      <c r="U23" s="43"/>
+      <c r="V23" s="43"/>
+      <c r="W23" s="44"/>
     </row>
     <row r="24" spans="1:23" ht="208.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="G24" s="30" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="32">
-        <v>2</v>
-      </c>
-      <c r="J24" s="43">
+      <c r="H24" s="27"/>
+      <c r="I24" s="28">
+        <v>2</v>
+      </c>
+      <c r="J24" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K24" s="44">
-        <v>1</v>
-      </c>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="7"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="7"/>
+      <c r="K24" s="31">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="3"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>